<commit_message>
prior revisions to file organization, add remainder of tocheck files.
</commit_message>
<xml_diff>
--- a/tocheck/temptnrsprob.xlsx
+++ b/tocheck/temptnrsprob.xlsx
@@ -743,7 +743,7 @@
         </is>
       </c>
       <c r="AW2" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="3">
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="AW3" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="4">
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="AW4" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="5">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="AW5" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="6">
@@ -1295,7 +1295,7 @@
         </is>
       </c>
       <c r="AW6" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="7">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="AW7" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="8">
@@ -1591,7 +1591,7 @@
         </is>
       </c>
       <c r="AW8" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="9">
@@ -1704,7 +1704,7 @@
         </is>
       </c>
       <c r="AW9" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="10">
@@ -1847,7 +1847,7 @@
         </is>
       </c>
       <c r="AW10" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="11">
@@ -1995,7 +1995,7 @@
         </is>
       </c>
       <c r="AW11" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="12">
@@ -2108,7 +2108,7 @@
         </is>
       </c>
       <c r="AW12" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="13">
@@ -2221,7 +2221,7 @@
         </is>
       </c>
       <c r="AW13" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="14">
@@ -2334,7 +2334,7 @@
         </is>
       </c>
       <c r="AW14" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="15">
@@ -2447,7 +2447,7 @@
         </is>
       </c>
       <c r="AW15" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="16">
@@ -2560,7 +2560,7 @@
         </is>
       </c>
       <c r="AW16" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="17">
@@ -2673,7 +2673,7 @@
         </is>
       </c>
       <c r="AW17" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
     <row r="18">
@@ -2821,7 +2821,7 @@
         </is>
       </c>
       <c r="AW18" s="2">
-        <v>45901</v>
+        <v>45905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>